<commit_message>
add one entry to frequently_occurring_artists_of_recordings_withReconciledWikiID
</commit_message>
<xml_diff>
--- a/thesession/data/reconciled/reconciledEntries/frequently_occurring_artists_of_recordings_withReconciledWikiID.xlsx
+++ b/thesession/data/reconciled/reconciledEntries/frequently_occurring_artists_of_recordings_withReconciledWikiID.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29620" windowHeight="13660"/>
+    <workbookView windowHeight="13040"/>
   </bookViews>
   <sheets>
     <sheet name="topFrequentlyOccuringArtists" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="185">
   <si>
     <t>Artist</t>
   </si>
@@ -579,6 +579,12 @@
   </si>
   <si>
     <t>http://www.wikidata.org/entity/Q2080198</t>
+  </si>
+  <si>
+    <t>Adrienne Young</t>
+  </si>
+  <si>
+    <t>http://www.wikidata.org/entity/Q4685726</t>
   </si>
 </sst>
 </file>
@@ -1755,12 +1761,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96:B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
@@ -1954,7 +1960,6 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13"/>
       <c r="F13" t="s">
         <v>31</v>
       </c>
@@ -2596,8 +2601,16 @@
       <c r="A95" t="s">
         <v>181</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>183</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2689,6 +2702,8 @@
     <hyperlink ref="B14" r:id="rId82" display="http://www.wikidata.org/entity/Q7490578"/>
     <hyperlink ref="B15" r:id="rId83" display="http://www.wikidata.org/entity/Q1271501"/>
     <hyperlink ref="B16" r:id="rId84" display="http://www.wikidata.org/entity/Q1179823"/>
+    <hyperlink ref="B95" r:id="rId85" display="http://www.wikidata.org/entity/Q2080198"/>
+    <hyperlink ref="B96" r:id="rId86" display="http://www.wikidata.org/entity/Q4685726"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update the manually reconciled list for artists of TheSession
</commit_message>
<xml_diff>
--- a/thesession/data/reconciled/reconciledEntries/frequently_occurring_artists_of_recordings_withReconciledWikiID.xlsx
+++ b/thesession/data/reconciled/reconciledEntries/frequently_occurring_artists_of_recordings_withReconciledWikiID.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="19100"/>
+    <workbookView windowWidth="28000" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="topFrequentlyOccuringArtists" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">topFrequentlyOccuringArtists!$A$1:$G$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">topFrequentlyOccuringArtists!$A$1:$G$96</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -625,6 +625,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -635,14 +643,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1079,28 +1079,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1224,14 +1224,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1775,7 +1778,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -1841,7 +1844,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
@@ -1858,7 +1861,7 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
@@ -1884,7 +1887,7 @@
       <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>2950</v>
       </c>
     </row>
@@ -1909,7 +1912,7 @@
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
@@ -1918,7 +1921,7 @@
       <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>26463</v>
       </c>
       <c r="H8" t="s">
@@ -1957,7 +1960,7 @@
       <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>20143</v>
       </c>
     </row>
@@ -1996,7 +1999,7 @@
       <c r="A14" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C14" t="s">
@@ -2007,7 +2010,7 @@
       <c r="A15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C15" t="s">
@@ -2021,7 +2024,7 @@
       <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C16" t="s">
@@ -2074,7 +2077,7 @@
       <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2629,7 +2632,7 @@
       <c r="A95" t="s">
         <v>184</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="3" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2637,12 +2640,12 @@
       <c r="A96" t="s">
         <v>186</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="3" t="s">
         <v>187</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G95">
+  <autoFilter ref="A1:G96">
     <extLst/>
   </autoFilter>
   <hyperlinks>

</xml_diff>